<commit_message>
made table for results page
made via excel lol
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/winsontruong/Documents/GitHub/police/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1E6C87-C591-0442-91A1-22D21D379F6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24462EE3-EF06-6545-A219-C44759007460}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4600" windowWidth="28800" windowHeight="16440" xr2:uid="{086A741B-C705-064C-8AFD-89718DDE3A33}"/>
   </bookViews>
@@ -519,7 +519,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>